<commit_message>
Updated with best results
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abhii\Source\Repos\branchprediction\source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abhii\Source\Repos\branchprediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -440,11 +440,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M8" sqref="M8"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -504,7 +504,7 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>12.856</v>
+        <v>12.778</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
@@ -522,7 +522,7 @@
         <v>5</v>
       </c>
       <c r="L3">
-        <v>12.741</v>
+        <v>12.39</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -530,7 +530,7 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>11.007</v>
+        <v>9.9309999999999992</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -542,13 +542,13 @@
         <v>6</v>
       </c>
       <c r="I4">
-        <v>7.99</v>
+        <v>7.9870000000000001</v>
       </c>
       <c r="K4" t="s">
         <v>6</v>
       </c>
       <c r="L4">
-        <v>10.257999999999999</v>
+        <v>9.5719999999999992</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
@@ -556,7 +556,7 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>9.5410000000000004</v>
+        <v>8.4600000000000009</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -574,7 +574,7 @@
         <v>7</v>
       </c>
       <c r="L5">
-        <v>8.4160000000000004</v>
+        <v>7.3739999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
@@ -582,7 +582,7 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>9.4879999999999995</v>
+        <v>7.492</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -594,13 +594,13 @@
         <v>8</v>
       </c>
       <c r="I6">
-        <v>6.0590000000000002</v>
+        <v>5.351</v>
       </c>
       <c r="K6" t="s">
         <v>8</v>
       </c>
       <c r="L6">
-        <v>6.7279999999999998</v>
+        <v>5.8730000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
@@ -608,25 +608,25 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>8.3879999999999999</v>
+        <v>6.7140000000000004</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
       </c>
       <c r="F7">
-        <v>7.5330000000000004</v>
+        <v>7.5529999999999999</v>
       </c>
       <c r="H7" t="s">
         <v>9</v>
       </c>
       <c r="I7">
-        <v>4.7850000000000001</v>
+        <v>3.1419999999999999</v>
       </c>
       <c r="K7" t="s">
         <v>9</v>
       </c>
       <c r="L7">
-        <v>5.3319999999999999</v>
+        <v>4.8840000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
@@ -634,7 +634,7 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>5.5670000000000002</v>
+        <v>5.1950000000000003</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -646,490 +646,490 @@
         <v>10</v>
       </c>
       <c r="I8">
-        <v>3.6869999999999998</v>
+        <v>1.3420000000000001</v>
       </c>
       <c r="K8" t="s">
         <v>10</v>
       </c>
       <c r="L8">
-        <v>3.706</v>
+        <v>3.1480000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>3.3690000000000002</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>4.4429999999999996</v>
+      </c>
+      <c r="H10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>3.496</v>
+      </c>
+      <c r="K10" t="s">
+        <v>5</v>
+      </c>
+      <c r="L10">
+        <v>3.27</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>3.5510000000000002</v>
+        <v>2.956</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F11">
-        <v>4.4429999999999996</v>
+        <v>4.298</v>
       </c>
       <c r="H11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I11">
-        <v>4.7140000000000004</v>
+        <v>3.3359999999999999</v>
       </c>
       <c r="K11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L11">
-        <v>3.641</v>
+        <v>2.8719999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12">
-        <v>2.956</v>
+        <v>2.7010000000000001</v>
       </c>
       <c r="E12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F12">
-        <v>4.298</v>
+        <v>4.1310000000000002</v>
       </c>
       <c r="H12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I12">
-        <v>3.3359999999999999</v>
+        <v>2.5950000000000002</v>
       </c>
       <c r="K12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L12">
-        <v>3.278</v>
+        <v>2.629</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C13">
-        <v>2.7010000000000001</v>
+        <v>2.665</v>
       </c>
       <c r="E13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F13">
-        <v>4.1310000000000002</v>
+        <v>3.8380000000000001</v>
       </c>
       <c r="H13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I13">
-        <v>3.2559999999999998</v>
+        <v>2.282</v>
       </c>
       <c r="K13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L13">
-        <v>2.7069999999999999</v>
+        <v>2.4660000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C14">
-        <v>2.7010000000000001</v>
+        <v>2.6360000000000001</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F14">
-        <v>3.8380000000000001</v>
+        <v>3.6760000000000002</v>
       </c>
       <c r="H14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I14">
-        <v>3.2360000000000002</v>
+        <v>2.0510000000000002</v>
       </c>
       <c r="K14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L14">
-        <v>2.4660000000000002</v>
+        <v>2.4409999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C15">
-        <v>2.6360000000000001</v>
+        <v>2.6339999999999999</v>
       </c>
       <c r="E15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F15">
-        <v>3.6760000000000002</v>
+        <v>3.3140000000000001</v>
       </c>
       <c r="H15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I15">
-        <v>2.7330000000000001</v>
+        <v>1.931</v>
       </c>
       <c r="K15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L15">
-        <v>2.4740000000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16">
-        <v>2.899</v>
-      </c>
-      <c r="E16" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16">
-        <v>3.3140000000000001</v>
-      </c>
-      <c r="H16" t="s">
-        <v>10</v>
-      </c>
-      <c r="I16">
-        <v>2.4950000000000001</v>
-      </c>
-      <c r="K16" t="s">
-        <v>10</v>
-      </c>
-      <c r="L16">
-        <v>2.4260000000000002</v>
+        <v>2.2959999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>10.912000000000001</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>10.151</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17">
+        <v>8.4640000000000004</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L17">
+        <v>10.416</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="B18" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C18">
-        <v>10.912000000000001</v>
+        <v>10.494</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F18">
-        <v>10.151</v>
+        <v>9.7100000000000009</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I18">
-        <v>8.4640000000000004</v>
+        <v>8.2040000000000006</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L18">
-        <v>11.138999999999999</v>
+        <v>9.8680000000000003</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C19">
-        <v>10.494</v>
+        <v>10.349</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F19">
-        <v>9.7100000000000009</v>
+        <v>9.4580000000000002</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I19">
-        <v>8.2319999999999993</v>
+        <v>7.8380000000000001</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L19">
-        <v>9.8680000000000003</v>
+        <v>9.3620000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C20">
-        <v>10.349</v>
+        <v>10.286</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F20">
-        <v>9.4580000000000002</v>
+        <v>9.2040000000000006</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I20">
-        <v>7.8380000000000001</v>
+        <v>7.6929999999999996</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L20">
-        <v>9.3620000000000001</v>
+        <v>9.0419999999999998</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B21" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C21">
-        <v>10.286</v>
+        <v>10.268000000000001</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F21">
-        <v>9.2040000000000006</v>
+        <v>9.0489999999999995</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I21">
-        <v>7.6929999999999996</v>
+        <v>7.5229999999999997</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L21">
-        <v>9.0419999999999998</v>
+        <v>8.8539999999999992</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B22" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C22">
         <v>10.268000000000001</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F22">
-        <v>9.0489999999999995</v>
+        <v>8.8840000000000003</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I22">
-        <v>7.5419999999999998</v>
+        <v>7.3630000000000004</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L22">
-        <v>9.0220000000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23">
-        <v>10.706</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23">
-        <v>8.9009999999999998</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I23">
-        <v>7.8840000000000003</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L23">
-        <v>8.5850000000000009</v>
+        <v>8.4629999999999992</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>11.509</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>13.766999999999999</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I24">
+        <v>12.6</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L24">
+        <v>11.613</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="B25" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C25">
-        <v>15.77</v>
+        <v>9.6370000000000005</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F25">
-        <v>13.766999999999999</v>
+        <v>10.699</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I25">
-        <v>12.621</v>
+        <v>10.148999999999999</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L25">
-        <v>12.86</v>
+        <v>9.5289999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B26" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C26">
-        <v>14.044</v>
+        <v>8.3030000000000008</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F26">
-        <v>10.699</v>
+        <v>7.6859999999999999</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I26">
-        <v>10.797000000000001</v>
+        <v>7.4349999999999996</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L26">
-        <v>12.236000000000001</v>
+        <v>7.4169999999999998</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B27" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C27">
-        <v>11.641</v>
+        <v>7.0839999999999996</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F27">
-        <v>7.6859999999999999</v>
+        <v>5.508</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I27">
-        <v>7.7809999999999997</v>
+        <v>4.9370000000000003</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L27">
-        <v>10.295</v>
+        <v>5.9429999999999996</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B28" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C28">
-        <v>9.11</v>
+        <v>6.0419999999999998</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F28">
-        <v>5.508</v>
+        <v>4.1379999999999999</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I28">
-        <v>4.9370000000000003</v>
+        <v>3.3</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L28">
-        <v>8.1720000000000006</v>
+        <v>4.8410000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B29" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C29">
-        <v>6.851</v>
+        <v>3.9159999999999999</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F29">
-        <v>4.1379999999999999</v>
+        <v>2.504</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I29">
-        <v>4.0640000000000001</v>
+        <v>2.0169999999999999</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L29">
-        <v>6.7939999999999996</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30">
-        <v>4.46</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30">
-        <v>2.504</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I30">
-        <v>2.2330000000000001</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L30">
-        <v>2.97</v>
+        <v>2.8130000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>